<commit_message>
emma and nate 10/3
</commit_message>
<xml_diff>
--- a/raw_ts_data/fd/fd3_ts1.xlsx
+++ b/raw_ts_data/fd/fd3_ts1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmaboudreau/Documents/GitHub/igea22/raw_ts_data/fd/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8AB9EC-5A69-9D4C-A0EE-36BCC771E508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97828AC1-9181-4F4A-A0FC-2548B49B9DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{EE1B1FB8-0281-4548-A9E5-3E5C43A73468}"/>
   </bookViews>
@@ -234,13 +234,13 @@
     <t>Location</t>
   </si>
   <si>
-    <t>X Section</t>
-  </si>
-  <si>
     <t>Reach</t>
   </si>
   <si>
     <t>PointID</t>
+  </si>
+  <si>
+    <t>XSection</t>
   </si>
 </sst>
 </file>
@@ -740,7 +740,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -756,13 +756,13 @@
     <row r="1" spans="1:8" s="19" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21"/>
       <c r="B1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>67</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>68</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>65</v>

</xml_diff>